<commit_message>
Updated graphics for dataset
</commit_message>
<xml_diff>
--- a/Project/data/data_raw_compiled.xlsx
+++ b/Project/data/data_raw_compiled.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="9">
   <si>
     <t>Maximum Frontier Size (number of Nodes)</t>
   </si>
@@ -40,6 +40,9 @@
   <si>
     <t>Total Number of Touched Nodes</t>
   </si>
+  <si>
+    <t>ORIGINAL DATA</t>
+  </si>
 </sst>
 </file>
 
@@ -49,7 +52,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -79,23 +82,20 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="8"/>
       <name val="TeX Gyre Bonum"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="TeX Gyre Bonum"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="9"/>
       <name val="TeX Gyre Bonum"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -107,12 +107,33 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -141,12 +162,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -222,7 +255,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -236,7 +269,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="800">
+              <a:rPr b="1" sz="800">
                 <a:latin typeface="TeX Gyre Bonum"/>
               </a:rPr>
               <a:t>Graph of Maximum Frontier Size for each algorithm </a:t>
@@ -276,7 +309,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -330,34 +363,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>0.004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>0.009</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28</c:v>
+                  <c:v>0.028</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>81</c:v>
+                  <c:v>0.081</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>244</c:v>
+                  <c:v>0.244</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>729</c:v>
+                  <c:v>0.729</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2188</c:v>
+                  <c:v>2.188</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6561</c:v>
+                  <c:v>6.561</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>19684</c:v>
+                  <c:v>19.684</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>59049</c:v>
+                  <c:v>59.049</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -389,7 +422,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -443,34 +476,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>0.003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>0.008</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21</c:v>
+                  <c:v>0.021</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>79</c:v>
+                  <c:v>0.079</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>254</c:v>
+                  <c:v>0.254</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1079</c:v>
+                  <c:v>1.079</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4247</c:v>
+                  <c:v>4.247</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16599</c:v>
+                  <c:v>16.599</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>66135</c:v>
+                  <c:v>66.135</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>262999</c:v>
+                  <c:v>262.999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -502,7 +535,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -556,34 +589,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>0.003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>0.014</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36</c:v>
+                  <c:v>0.036</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>156</c:v>
+                  <c:v>0.156</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>528</c:v>
+                  <c:v>0.528</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2164</c:v>
+                  <c:v>2.164</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8256</c:v>
+                  <c:v>8.256</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>33236</c:v>
+                  <c:v>33.236</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>131328</c:v>
+                  <c:v>131.328</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>526164</c:v>
+                  <c:v>526.164</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -615,7 +648,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -669,45 +702,45 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>0.005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>0.029</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>82</c:v>
+                  <c:v>0.082</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>245</c:v>
+                  <c:v>0.245</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>730</c:v>
+                  <c:v>0.73</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2189</c:v>
+                  <c:v>2.189</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6562</c:v>
+                  <c:v>6.562</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>19685</c:v>
+                  <c:v>19.685</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>59050</c:v>
+                  <c:v>59.05</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="4493710"/>
-        <c:axId val="14529378"/>
+        <c:axId val="56134735"/>
+        <c:axId val="92481174"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="4493710"/>
+        <c:axId val="56134735"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -732,7 +765,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900">
                     <a:latin typeface="TeX Gyre Bonum"/>
                   </a:rPr>
                   <a:t>Number of Disks</a:t>
@@ -752,14 +785,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="14529378"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="92481174"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="14529378"/>
+        <c:axId val="92481174"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -784,10 +817,10 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900">
                     <a:latin typeface="TeX Gyre Bonum"/>
                   </a:rPr>
-                  <a:t>Number of Nodes</a:t>
+                  <a:t>Number of Nodes (in thousands)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -804,8 +837,625 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="4493710"/>
+        <c:crossAx val="56134735"/>
         <c:crossesAt val="0"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1" sz="800">
+                <a:latin typeface="TeX Gyre Bonum"/>
+              </a:rPr>
+              <a:t>Graph of Runtime for each algorithm </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Depth_First_Search</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="6"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$16:$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$16:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.000156392000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.000204043999999987</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.000950633000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.00201636600000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.006868233</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.012976039</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0676599199999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.128477632999989</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.726265782999917</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.543463721</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bidirectional_BFS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="6"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$16:$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$16:$C$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.000212668999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.000455272000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00179459000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.00793697800000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.041572044</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.26530022</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.026069019</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.297773958</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>118.008149897</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>900.394615177</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Breadth_First_Search</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="6"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$16:$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$16:$D$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9.62859999999732E-005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.000719420999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00329481600000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01786741</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.106164721</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.740262595</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.571621341</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>52.629218872</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>389.933532058</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3774.456782876</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Iterative_Deepening_DFS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="579d1c"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="6"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$16:$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$16:$E$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.000472911999999992</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.000987642000000011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.009155311</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.055075039</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.537936986</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.933634893</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>55.269963468</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>744.907908745</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8319.07307241</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>84143.691529322</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="36943925"/>
+        <c:axId val="28358582"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="36943925"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900">
+                    <a:latin typeface="TeX Gyre Bonum"/>
+                  </a:rPr>
+                  <a:t>Number of Disks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="28358582"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="28358582"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900">
+                    <a:latin typeface="TeX Gyre Bonum"/>
+                  </a:rPr>
+                  <a:t>Total Runtime (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="36943925"/>
+        <c:crossesAt val="1"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -853,10 +1503,10 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="800">
+              <a:rPr b="1" sz="800">
                 <a:latin typeface="TeX Gyre Bonum"/>
               </a:rPr>
-              <a:t>Graph of Runtime for each algorithm </a:t>
+              <a:t>Graph of Traversed Nodes for each algorithm </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -872,7 +1522,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$15</c:f>
+              <c:f>Sheet1!$B$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -893,7 +1543,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -904,7 +1554,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$16:$A$25</c:f>
+              <c:f>Sheet1!$A$29:$A$38</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -942,39 +1592,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$16:$B$25</c:f>
+              <c:f>Sheet1!$B$29:$B$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.000156392000000005</c:v>
+                  <c:v>6E-006</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.000204043999999987</c:v>
+                  <c:v>9E-006</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.000950633000000006</c:v>
+                  <c:v>4.9E-005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.00201636600000002</c:v>
+                  <c:v>8.1E-005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.006868233</c:v>
+                  <c:v>0.000428</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.012976039</c:v>
+                  <c:v>0.000729</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0676599199999997</c:v>
+                  <c:v>0.003831</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.128477632999989</c:v>
+                  <c:v>0.006561</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.726265782999917</c:v>
+                  <c:v>0.03445</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.543463721</c:v>
+                  <c:v>0.059049</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -985,7 +1635,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$15</c:f>
+              <c:f>Sheet1!$C$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1006,7 +1656,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -1017,7 +1667,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$16:$A$25</c:f>
+              <c:f>Sheet1!$A$29:$A$38</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1055,39 +1705,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$C$25</c:f>
+              <c:f>Sheet1!$C$29:$C$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.000212668999999999</c:v>
+                  <c:v>1E-005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.000455272000000007</c:v>
+                  <c:v>2.2E-005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.00179459000000001</c:v>
+                  <c:v>8.6E-005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.00793697800000001</c:v>
+                  <c:v>0.000486</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.041572044</c:v>
+                  <c:v>0.002506</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.26530022</c:v>
+                  <c:v>0.015182</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.026069019</c:v>
+                  <c:v>0.091516</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16.297773958</c:v>
+                  <c:v>0.542326</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>118.008149897</c:v>
+                  <c:v>3.286532</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>900.394615177</c:v>
+                  <c:v>19.768542</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1098,7 +1748,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$15</c:f>
+              <c:f>Sheet1!$D$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1119,7 +1769,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -1130,7 +1780,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$16:$A$25</c:f>
+              <c:f>Sheet1!$A$29:$A$38</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1168,39 +1818,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$16:$D$25</c:f>
+              <c:f>Sheet1!$D$29:$D$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>9.62859999999732E-005</c:v>
+                  <c:v>5E-006</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.000719420999999998</c:v>
+                  <c:v>3.6E-005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.00329481600000001</c:v>
+                  <c:v>0.000184</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.01786741</c:v>
+                  <c:v>0.001194</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.106164721</c:v>
+                  <c:v>0.006738</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.740262595</c:v>
+                  <c:v>0.043288</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.571621341</c:v>
+                  <c:v>0.257792</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>52.629218872</c:v>
+                  <c:v>1.606086</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>389.933532058</c:v>
+                  <c:v>9.671326</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3774.456782876</c:v>
+                  <c:v>59.09634</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1211,7 +1861,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$15</c:f>
+              <c:f>Sheet1!$E$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1232,7 +1882,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -1243,7 +1893,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$16:$A$25</c:f>
+              <c:f>Sheet1!$A$29:$A$38</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1281,50 +1931,50 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$16:$E$25</c:f>
+              <c:f>Sheet1!$E$29:$E$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.000472911999999992</c:v>
+                  <c:v>2.8E-005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.000987642000000011</c:v>
+                  <c:v>5.5E-005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.009155311</c:v>
+                  <c:v>0.000534</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.055075039</c:v>
+                  <c:v>0.003403</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.537936986</c:v>
+                  <c:v>0.030992</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.933634893</c:v>
+                  <c:v>0.266815</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>55.269963468</c:v>
+                  <c:v>2.404618</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>744.907908745</c:v>
+                  <c:v>21.533203</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8319.07307241</c:v>
+                  <c:v>193.828356</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>84143.691529322</c:v>
+                  <c:v>1743.480775</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="95387286"/>
-        <c:axId val="2815244"/>
+        <c:axId val="34077266"/>
+        <c:axId val="11795336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95387286"/>
+        <c:axId val="34077266"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1349,7 +1999,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900">
                     <a:latin typeface="TeX Gyre Bonum"/>
                   </a:rPr>
                   <a:t>Number of Disks</a:t>
@@ -1369,14 +2019,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2815244"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="11795336"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2815244"/>
+        <c:axId val="11795336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1401,10 +2051,10 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900">
                     <a:latin typeface="TeX Gyre Bonum"/>
                   </a:rPr>
-                  <a:t>Total Runtime (seconds)</a:t>
+                  <a:t>Total Number of Traversed Nodes (in millions)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1421,624 +2071,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="95387286"/>
-        <c:crossesAt val="0"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr sz="800">
-                <a:latin typeface="TeX Gyre Bonum"/>
-              </a:rPr>
-              <a:t>Graph of Traversed Nodes for each algorithm </a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$28</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Depth_First_Search</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:size val="7"/>
-          </c:marker>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$29:$A$38</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$29:$B$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>428</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>729</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3831</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6561</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>34450</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>59049</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$28</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Bidirectional_BFS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ff420e"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:size val="7"/>
-          </c:marker>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$29:$A$38</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$29:$C$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>86</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>486</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2506</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>15182</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>91516</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>542326</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3286532</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>19768542</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$28</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Breadth_First_Search</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ffd320"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:size val="7"/>
-          </c:marker>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$29:$A$38</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$29:$D$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>184</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1194</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6738</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43288</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>257792</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1606086</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9671326</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>59096340</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$28</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Iterative_Deepening_DFS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="579d1c"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:size val="7"/>
-          </c:marker>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$29:$A$38</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$E$29:$E$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>534</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3403</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>30992</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>266815</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2404618</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>21533203</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>193828356</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1743480775</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="81544772"/>
-        <c:axId val="94137202"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="81544772"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr sz="900">
-                    <a:latin typeface="TeX Gyre Bonum"/>
-                  </a:rPr>
-                  <a:t>Number of Disks</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="94137202"/>
-        <c:crossesAt val="0"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="94137202"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr sz="900">
-                    <a:latin typeface="TeX Gyre Bonum"/>
-                  </a:rPr>
-                  <a:t>Total Number of Traversed Nodes</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="81544772"/>
+        <c:crossAx val="34077266"/>
         <c:crossesAt val="1"/>
       </c:valAx>
       <c:spPr>
@@ -2078,15 +2111,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>33840</xdr:colOff>
+      <xdr:colOff>43920</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>153000</xdr:rowOff>
+      <xdr:rowOff>143280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>219600</xdr:colOff>
+      <xdr:colOff>249120</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>95760</xdr:rowOff>
+      <xdr:rowOff>86400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2094,8 +2127,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7184520" y="153000"/>
-        <a:ext cx="4249800" cy="4006440"/>
+        <a:off x="7194600" y="143280"/>
+        <a:ext cx="4269240" cy="4006800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2108,15 +2141,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>24480</xdr:colOff>
+      <xdr:colOff>51480</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>210240</xdr:colOff>
+      <xdr:colOff>236880</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>115560</xdr:rowOff>
+      <xdr:rowOff>106200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2124,8 +2157,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7175160" y="4399560"/>
-        <a:ext cx="4249800" cy="4006440"/>
+        <a:off x="7202160" y="4390560"/>
+        <a:ext cx="4249440" cy="4006080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2138,15 +2171,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1004400</xdr:colOff>
+      <xdr:colOff>1001880</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>48960</xdr:rowOff>
+      <xdr:rowOff>39960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1539720</xdr:colOff>
+      <xdr:colOff>1536840</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>153720</xdr:rowOff>
+      <xdr:rowOff>144360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2154,8 +2187,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2066040" y="6713640"/>
-        <a:ext cx="4249800" cy="4006440"/>
+        <a:off x="2063520" y="6704640"/>
+        <a:ext cx="4249440" cy="4006080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2173,10 +2206,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:M110"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2193,6 +2226,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="M1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -2210,181 +2244,196 @@
       <c r="E2" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="M2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>4</v>
+        <v>0.004</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>3</v>
+        <v>0.003</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>3</v>
+        <v>0.003</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>5</v>
-      </c>
+        <v>0.005</v>
+      </c>
+      <c r="M3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>9</v>
+        <v>0.009</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>8</v>
+        <v>0.008</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>14</v>
+        <v>0.014</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>10</v>
-      </c>
+        <v>0.01</v>
+      </c>
+      <c r="M4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>28</v>
+        <v>0.028</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>21</v>
+        <v>0.021</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>36</v>
+        <v>0.036</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>29</v>
-      </c>
+        <v>0.029</v>
+      </c>
+      <c r="M5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>81</v>
+        <v>0.081</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>79</v>
+        <v>0.079</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>156</v>
+        <v>0.156</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>82</v>
-      </c>
+        <v>0.082</v>
+      </c>
+      <c r="M6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>244</v>
+        <v>0.244</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>254</v>
+        <v>0.254</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>528</v>
+        <v>0.528</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>245</v>
-      </c>
+        <v>0.245</v>
+      </c>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>729</v>
+        <v>0.729</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>1079</v>
+        <v>1.079</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>2164</v>
+        <v>2.164</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>730</v>
-      </c>
+        <v>0.73</v>
+      </c>
+      <c r="M8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>2188</v>
+        <v>2.188</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>4247</v>
+        <v>4.247</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>8256</v>
+        <v>8.256</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>2189</v>
-      </c>
+        <v>2.189</v>
+      </c>
+      <c r="M9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>6561</v>
+        <v>6.561</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>16599</v>
+        <v>16.599</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>33236</v>
+        <v>33.236</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>6562</v>
-      </c>
+        <v>6.562</v>
+      </c>
+      <c r="M10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>19684</v>
+        <v>19.684</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>66135</v>
+        <v>66.135</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>131328</v>
+        <v>131.328</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>19685</v>
-      </c>
+        <v>19.685</v>
+      </c>
+      <c r="M11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>59049</v>
+        <v>59.049</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>262999</v>
+        <v>262.999</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>526164</v>
+        <v>526.164</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>59050</v>
-      </c>
+        <v>59.05</v>
+      </c>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="M14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
@@ -2402,6 +2451,7 @@
       <c r="E15" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="M15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -2419,6 +2469,7 @@
       <c r="E16" s="0" t="n">
         <v>0.000472911999999992</v>
       </c>
+      <c r="M16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
@@ -2436,6 +2487,7 @@
       <c r="E17" s="0" t="n">
         <v>0.000987642000000011</v>
       </c>
+      <c r="M17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -2453,6 +2505,7 @@
       <c r="E18" s="0" t="n">
         <v>0.009155311</v>
       </c>
+      <c r="M18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
@@ -2470,6 +2523,7 @@
       <c r="E19" s="0" t="n">
         <v>0.055075039</v>
       </c>
+      <c r="M19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -2487,6 +2541,7 @@
       <c r="E20" s="0" t="n">
         <v>0.537936986</v>
       </c>
+      <c r="M20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
@@ -2504,6 +2559,7 @@
       <c r="E21" s="0" t="n">
         <v>4.933634893</v>
       </c>
+      <c r="M21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -2521,6 +2577,7 @@
       <c r="E22" s="0" t="n">
         <v>55.269963468</v>
       </c>
+      <c r="M22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -2538,6 +2595,7 @@
       <c r="E23" s="0" t="n">
         <v>744.907908745</v>
       </c>
+      <c r="M23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
@@ -2555,6 +2613,7 @@
       <c r="E24" s="0" t="n">
         <v>8319.07307241</v>
       </c>
+      <c r="M24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
@@ -2572,11 +2631,16 @@
       <c r="E25" s="0" t="n">
         <v>84143.691529322</v>
       </c>
+      <c r="M25" s="2"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="M27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
@@ -2594,174 +2658,871 @@
       <c r="E28" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="M28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>6</v>
+        <v>6E-006</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>10</v>
+        <v>1E-005</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>5</v>
+        <v>5E-006</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>28</v>
-      </c>
+        <v>2.8E-005</v>
+      </c>
+      <c r="M29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>9</v>
+        <v>9E-006</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>22</v>
+        <v>2.2E-005</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>36</v>
+        <v>3.6E-005</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>55</v>
-      </c>
+        <v>5.5E-005</v>
+      </c>
+      <c r="M30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>49</v>
+        <v>4.9E-005</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>86</v>
+        <v>8.6E-005</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>184</v>
+        <v>0.000184</v>
       </c>
       <c r="E31" s="0" t="n">
-        <v>534</v>
-      </c>
+        <v>0.000534</v>
+      </c>
+      <c r="M31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>5</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>81</v>
+        <v>8.1E-005</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>486</v>
+        <v>0.000486</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>1194</v>
+        <v>0.001194</v>
       </c>
       <c r="E32" s="0" t="n">
-        <v>3403</v>
-      </c>
+        <v>0.003403</v>
+      </c>
+      <c r="M32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>6</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>428</v>
+        <v>0.000428</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>2506</v>
+        <v>0.002506</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>6738</v>
+        <v>0.006738</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>30992</v>
-      </c>
+        <v>0.030992</v>
+      </c>
+      <c r="M33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>7</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>729</v>
+        <v>0.000729</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>15182</v>
+        <v>0.015182</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>43288</v>
+        <v>0.043288</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>266815</v>
-      </c>
+        <v>0.266815</v>
+      </c>
+      <c r="M34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>8</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>3831</v>
+        <v>0.003831</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>91516</v>
+        <v>0.091516</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>257792</v>
+        <v>0.257792</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>2404618</v>
-      </c>
+        <v>2.404618</v>
+      </c>
+      <c r="M35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <v>9</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>6561</v>
+        <v>0.006561</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>542326</v>
+        <v>0.542326</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>1606086</v>
+        <v>1.606086</v>
       </c>
       <c r="E36" s="0" t="n">
-        <v>21533203</v>
-      </c>
+        <v>21.533203</v>
+      </c>
+      <c r="M36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <v>10</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>34450</v>
+        <v>0.03445</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>3286532</v>
+        <v>3.286532</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>9671326</v>
+        <v>9.671326</v>
       </c>
       <c r="E37" s="0" t="n">
-        <v>193828356</v>
-      </c>
+        <v>193.828356</v>
+      </c>
+      <c r="M37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <v>11</v>
       </c>
       <c r="B38" s="0" t="n">
+        <v>0.059049</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>19.768542</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>59.09634</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>1743.480775</v>
+      </c>
+      <c r="M38" s="2"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M39" s="2"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M40" s="2"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M41" s="2"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M42" s="2"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M43" s="2"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M44" s="2"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M45" s="2"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M46" s="2"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M47" s="2"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M48" s="2"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M49" s="2"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M50" s="2"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M51" s="2"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M52" s="2"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M53" s="2"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M54" s="2"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M55" s="2"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M56" s="2"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M57" s="2"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M58" s="2"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M59" s="2"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M60" s="2"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M61" s="2"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M62" s="2"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M63" s="2"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M64" s="2"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M65" s="2"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M66" s="2"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M67" s="2"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M68" s="2"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3"/>
+      <c r="J69" s="3"/>
+      <c r="K69" s="3"/>
+      <c r="L69" s="3"/>
+      <c r="M69" s="4"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E74" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B75" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C75" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D75" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E75" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B76" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C76" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D76" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="E76" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B77" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C77" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="E77" s="0" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B78" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="C78" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>156</v>
+      </c>
+      <c r="E78" s="0" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B79" s="0" t="n">
+        <v>244</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <v>254</v>
+      </c>
+      <c r="D79" s="0" t="n">
+        <v>528</v>
+      </c>
+      <c r="E79" s="0" t="n">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B80" s="0" t="n">
+        <v>729</v>
+      </c>
+      <c r="C80" s="0" t="n">
+        <v>1079</v>
+      </c>
+      <c r="D80" s="0" t="n">
+        <v>2164</v>
+      </c>
+      <c r="E80" s="0" t="n">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B81" s="0" t="n">
+        <v>2188</v>
+      </c>
+      <c r="C81" s="0" t="n">
+        <v>4247</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>8256</v>
+      </c>
+      <c r="E81" s="0" t="n">
+        <v>2189</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B82" s="0" t="n">
+        <v>6561</v>
+      </c>
+      <c r="C82" s="0" t="n">
+        <v>16599</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>33236</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <v>6562</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B83" s="0" t="n">
+        <v>19684</v>
+      </c>
+      <c r="C83" s="0" t="n">
+        <v>66135</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>131328</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <v>19685</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B84" s="0" t="n">
         <v>59049</v>
       </c>
-      <c r="C38" s="0" t="n">
+      <c r="C84" s="0" t="n">
+        <v>262999</v>
+      </c>
+      <c r="D84" s="0" t="n">
+        <v>526164</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <v>59050</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D87" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E87" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B88" s="0" t="n">
+        <v>0.000156392000000005</v>
+      </c>
+      <c r="C88" s="0" t="n">
+        <v>0.000212668999999999</v>
+      </c>
+      <c r="D88" s="0" t="n">
+        <v>9.62859999999732E-005</v>
+      </c>
+      <c r="E88" s="0" t="n">
+        <v>0.000472911999999992</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B89" s="0" t="n">
+        <v>0.000204043999999987</v>
+      </c>
+      <c r="C89" s="0" t="n">
+        <v>0.000455272000000007</v>
+      </c>
+      <c r="D89" s="0" t="n">
+        <v>0.000719420999999998</v>
+      </c>
+      <c r="E89" s="0" t="n">
+        <v>0.000987642000000011</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B90" s="0" t="n">
+        <v>0.000950633000000006</v>
+      </c>
+      <c r="C90" s="0" t="n">
+        <v>0.00179459000000001</v>
+      </c>
+      <c r="D90" s="0" t="n">
+        <v>0.00329481600000001</v>
+      </c>
+      <c r="E90" s="0" t="n">
+        <v>0.009155311</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B91" s="0" t="n">
+        <v>0.00201636600000002</v>
+      </c>
+      <c r="C91" s="0" t="n">
+        <v>0.00793697800000001</v>
+      </c>
+      <c r="D91" s="0" t="n">
+        <v>0.01786741</v>
+      </c>
+      <c r="E91" s="0" t="n">
+        <v>0.055075039</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B92" s="0" t="n">
+        <v>0.006868233</v>
+      </c>
+      <c r="C92" s="0" t="n">
+        <v>0.041572044</v>
+      </c>
+      <c r="D92" s="0" t="n">
+        <v>0.106164721</v>
+      </c>
+      <c r="E92" s="0" t="n">
+        <v>0.537936986</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B93" s="0" t="n">
+        <v>0.012976039</v>
+      </c>
+      <c r="C93" s="0" t="n">
+        <v>0.26530022</v>
+      </c>
+      <c r="D93" s="0" t="n">
+        <v>0.740262595</v>
+      </c>
+      <c r="E93" s="0" t="n">
+        <v>4.933634893</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B94" s="0" t="n">
+        <v>0.0676599199999997</v>
+      </c>
+      <c r="C94" s="0" t="n">
+        <v>2.026069019</v>
+      </c>
+      <c r="D94" s="0" t="n">
+        <v>6.571621341</v>
+      </c>
+      <c r="E94" s="0" t="n">
+        <v>55.269963468</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B95" s="0" t="n">
+        <v>0.128477632999989</v>
+      </c>
+      <c r="C95" s="0" t="n">
+        <v>16.297773958</v>
+      </c>
+      <c r="D95" s="0" t="n">
+        <v>52.629218872</v>
+      </c>
+      <c r="E95" s="0" t="n">
+        <v>744.907908745</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B96" s="0" t="n">
+        <v>0.726265782999917</v>
+      </c>
+      <c r="C96" s="0" t="n">
+        <v>118.008149897</v>
+      </c>
+      <c r="D96" s="0" t="n">
+        <v>389.933532058</v>
+      </c>
+      <c r="E96" s="0" t="n">
+        <v>8319.07307241</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B97" s="0" t="n">
+        <v>1.543463721</v>
+      </c>
+      <c r="C97" s="0" t="n">
+        <v>900.394615177</v>
+      </c>
+      <c r="D97" s="0" t="n">
+        <v>3774.456782876</v>
+      </c>
+      <c r="E97" s="0" t="n">
+        <v>84143.691529322</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C100" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D100" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E100" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B101" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C101" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D101" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E101" s="0" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B102" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C102" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="D102" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="E102" s="0" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B103" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="C103" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="D103" s="0" t="n">
+        <v>184</v>
+      </c>
+      <c r="E103" s="0" t="n">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B104" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="C104" s="0" t="n">
+        <v>486</v>
+      </c>
+      <c r="D104" s="0" t="n">
+        <v>1194</v>
+      </c>
+      <c r="E104" s="0" t="n">
+        <v>3403</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B105" s="0" t="n">
+        <v>428</v>
+      </c>
+      <c r="C105" s="0" t="n">
+        <v>2506</v>
+      </c>
+      <c r="D105" s="0" t="n">
+        <v>6738</v>
+      </c>
+      <c r="E105" s="0" t="n">
+        <v>30992</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B106" s="0" t="n">
+        <v>729</v>
+      </c>
+      <c r="C106" s="0" t="n">
+        <v>15182</v>
+      </c>
+      <c r="D106" s="0" t="n">
+        <v>43288</v>
+      </c>
+      <c r="E106" s="0" t="n">
+        <v>266815</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B107" s="0" t="n">
+        <v>3831</v>
+      </c>
+      <c r="C107" s="0" t="n">
+        <v>91516</v>
+      </c>
+      <c r="D107" s="0" t="n">
+        <v>257792</v>
+      </c>
+      <c r="E107" s="0" t="n">
+        <v>2404618</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B108" s="0" t="n">
+        <v>6561</v>
+      </c>
+      <c r="C108" s="0" t="n">
+        <v>542326</v>
+      </c>
+      <c r="D108" s="0" t="n">
+        <v>1606086</v>
+      </c>
+      <c r="E108" s="0" t="n">
+        <v>21533203</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B109" s="0" t="n">
+        <v>34450</v>
+      </c>
+      <c r="C109" s="0" t="n">
+        <v>3286532</v>
+      </c>
+      <c r="D109" s="0" t="n">
+        <v>9671326</v>
+      </c>
+      <c r="E109" s="0" t="n">
+        <v>193828356</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B110" s="0" t="n">
+        <v>59049</v>
+      </c>
+      <c r="C110" s="0" t="n">
         <v>19768542</v>
       </c>
-      <c r="D38" s="0" t="n">
+      <c r="D110" s="0" t="n">
         <v>59096340</v>
       </c>
-      <c r="E38" s="0" t="n">
+      <c r="E110" s="0" t="n">
         <v>1743480775</v>
       </c>
     </row>

</xml_diff>